<commit_message>
[Added] Overtime Computer in HourProcessor.cs [Fixed] Holiday Checker in HourProcessor.cs
</commit_message>
<xml_diff>
--- a/HourCompuationTable.xlsx
+++ b/HourCompuationTable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
   <si>
     <t>Sunday</t>
   </si>
@@ -210,13 +210,22 @@
   </si>
   <si>
     <t>sun_overtime_night_regular</t>
+  </si>
+  <si>
+    <t>HourProcessor.cs</t>
+  </si>
+  <si>
+    <t>overtime</t>
+  </si>
+  <si>
+    <t>actual duty needed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,8 +254,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,6 +333,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -332,29 +361,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
@@ -378,6 +392,28 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -663,302 +699,397 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:AH13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.875" customWidth="1"/>
-    <col min="2" max="10" width="25.875" customWidth="1"/>
-    <col min="11" max="15" width="13.375" customWidth="1"/>
+    <col min="2" max="8" width="25.875" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
+    <col min="10" max="38" width="2.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="3" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="2" t="s">
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="15"/>
+      <c r="B2" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="4" t="s">
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="16" t="s">
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="15"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="6" t="s">
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="K3">
+        <v>7</v>
+      </c>
+      <c r="L3">
+        <v>8</v>
+      </c>
+      <c r="M3">
+        <v>9</v>
+      </c>
+      <c r="N3">
+        <v>10</v>
+      </c>
+      <c r="O3">
+        <v>11</v>
+      </c>
+      <c r="P3">
+        <v>12</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>2</v>
+      </c>
+      <c r="S3">
+        <v>3</v>
+      </c>
+      <c r="T3">
+        <v>4</v>
+      </c>
+      <c r="U3">
         <v>5</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="V3">
+        <v>6</v>
+      </c>
+      <c r="W3">
+        <v>7</v>
+      </c>
+      <c r="X3">
+        <v>8</v>
+      </c>
+      <c r="Y3">
+        <v>9</v>
+      </c>
+      <c r="Z3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="7" t="s">
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="L5" s="26"/>
+      <c r="M5" s="26"/>
+      <c r="N5" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="O5" s="26"/>
+      <c r="P5" s="26"/>
+      <c r="Q5" s="26"/>
+      <c r="R5" s="26"/>
+      <c r="S5" s="26"/>
+      <c r="T5" s="26"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="21" t="s">
+      <c r="C6" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="F6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="H6" s="21" t="s">
+      <c r="H6" s="18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="17"/>
-      <c r="B7" s="15" t="s">
+      <c r="L6" s="27"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="27"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="R6" s="27"/>
+      <c r="S6" s="27"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="27"/>
+      <c r="Y6" s="27"/>
+      <c r="Z6" s="27"/>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="12"/>
+      <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="16">
         <v>1</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="16">
         <v>1.3</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="16">
         <v>2</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="16">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="16" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="18"/>
-      <c r="B9" s="13" t="s">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="22">
+      <c r="C9" s="17">
         <v>1.25</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="21" t="s">
+      <c r="H10" s="18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="15" t="s">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="14"/>
+      <c r="B11" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="16">
         <v>1.3</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="16">
         <v>1.5</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="16">
         <v>2.6</v>
       </c>
-      <c r="F11" s="21" t="s">
+      <c r="F11" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="21" t="s">
+      <c r="H11" s="16" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="22" t="s">
+      <c r="D12" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
-      <c r="B13" s="13" t="s">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="23"/>
+      <c r="B13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="17" t="s">
         <v>49</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Added] Payroll Computations [Added] Pay rates definitions [Added] Initialized hour and rates.
</commit_message>
<xml_diff>
--- a/HourCompuationTable.xlsx
+++ b/HourCompuationTable.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
   <si>
     <t>Sunday</t>
   </si>
@@ -134,48 +134,6 @@
     <t>nsu_proper_night_regular</t>
   </si>
   <si>
-    <t>1.3 * 1.1</t>
-  </si>
-  <si>
-    <t>2 * 1.1</t>
-  </si>
-  <si>
-    <t>1.5 * 1.1</t>
-  </si>
-  <si>
-    <t>2.6 * 1.1</t>
-  </si>
-  <si>
-    <t>1.3 * 1.3</t>
-  </si>
-  <si>
-    <t>2 * 1.3</t>
-  </si>
-  <si>
-    <t>1.1* 1.25</t>
-  </si>
-  <si>
-    <t>1.3 * 1.1 * 1.3</t>
-  </si>
-  <si>
-    <t>2 * 1.1 * 1.3</t>
-  </si>
-  <si>
-    <t>1.5 * 1.3</t>
-  </si>
-  <si>
-    <t>2.6 * 1.3</t>
-  </si>
-  <si>
-    <t>1.3 * 1.25</t>
-  </si>
-  <si>
-    <t>1.5 * 1.1 * 1.3</t>
-  </si>
-  <si>
-    <t>2.6 * 1.1 * 1.3</t>
-  </si>
-  <si>
     <t>nsu_overtime_day_normal</t>
   </si>
   <si>
@@ -219,6 +177,51 @@
   </si>
   <si>
     <t>actual duty needed</t>
+  </si>
+  <si>
+    <t>1 = 1</t>
+  </si>
+  <si>
+    <t>1.3 * 1.1 = 1.43</t>
+  </si>
+  <si>
+    <t>2 * 1.1 = 2.2</t>
+  </si>
+  <si>
+    <t>1.3 * 1.3 = 1.69</t>
+  </si>
+  <si>
+    <t>2 * 1.3 = 2.6</t>
+  </si>
+  <si>
+    <t>1.1* 1.25 = 1.375</t>
+  </si>
+  <si>
+    <t>1.3 * 1.1 * 1.3 = 1.859</t>
+  </si>
+  <si>
+    <t>2 * 1.1 * 1.3 = 2.86</t>
+  </si>
+  <si>
+    <t>1.5 * 1.1 = 1.65</t>
+  </si>
+  <si>
+    <t>2.6 * 1.1 = 2.86</t>
+  </si>
+  <si>
+    <t>1.3 * 1.25 = 1.625</t>
+  </si>
+  <si>
+    <t>1.5 * 1.3= 1.95</t>
+  </si>
+  <si>
+    <t>2.6 * 1.3 = 3.38</t>
+  </si>
+  <si>
+    <t>1.5 * 1.1 * 1.3 = 2.145</t>
+  </si>
+  <si>
+    <t>2.6 * 1.1 * 1.3 = 3.718</t>
   </si>
 </sst>
 </file>
@@ -395,6 +398,10 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -410,10 +417,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -699,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH13"/>
+  <dimension ref="A1:Z13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X12" sqref="X12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,32 +719,32 @@
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
       <c r="B1" s="15"/>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="22" t="s">
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
       <c r="B2" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="21" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
@@ -826,22 +829,22 @@
       <c r="H4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
-      <c r="R4" s="25"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="25"/>
-      <c r="U4" s="25"/>
-      <c r="V4" s="25"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="24"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+      <c r="S4" s="20"/>
+      <c r="T4" s="20"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="20"/>
+      <c r="W4" s="19"/>
+      <c r="X4" s="19"/>
+      <c r="Y4" s="19"/>
+      <c r="Z4" s="19"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
@@ -864,17 +867,17 @@
       <c r="H5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
-      <c r="N5" s="26" t="s">
-        <v>64</v>
-      </c>
-      <c r="O5" s="26"/>
-      <c r="P5" s="26"/>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
@@ -901,31 +904,31 @@
       <c r="H6" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="R6" s="27"/>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="27"/>
-      <c r="V6" s="27"/>
-      <c r="W6" s="27"/>
-      <c r="X6" s="27"/>
-      <c r="Y6" s="27"/>
-      <c r="Z6" s="27"/>
+      <c r="L6" s="22"/>
+      <c r="M6" s="22"/>
+      <c r="N6" s="22"/>
+      <c r="O6" s="22"/>
+      <c r="P6" s="22"/>
+      <c r="Q6" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="R6" s="22"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="22"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="22"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
+      <c r="Y6" s="22"/>
+      <c r="Z6" s="22"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="12"/>
       <c r="B7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="16">
-        <v>1</v>
+      <c r="C7" s="16" t="s">
+        <v>51</v>
       </c>
       <c r="D7" s="16">
         <v>1.3</v>
@@ -937,10 +940,10 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.25">
@@ -951,22 +954,22 @@
         <v>16</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="H8" s="17" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.25">
@@ -978,19 +981,19 @@
         <v>1.25</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.25">
@@ -1034,63 +1037,63 @@
         <v>2.6</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="27" t="s">
         <v>17</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="F12" s="17" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A13" s="23"/>
+      <c r="A13" s="27"/>
       <c r="B13" s="8" t="s">
         <v>22</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HourProcessor.cs:  fields changed to dictionary. Compute Hours now working.
</commit_message>
<xml_diff>
--- a/HourCompuationTable.xlsx
+++ b/HourCompuationTable.xlsx
@@ -702,10 +702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z13"/>
+  <dimension ref="A1:Z40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="95" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1096,6 +1096,126 @@
         <v>65</v>
       </c>
     </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <v>1.69</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>1.859</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>1.65</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>1.625</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>1.859</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>2.145</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>3.718</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="C2:E2"/>

</xml_diff>